<commit_message>
Correção no nome da coluna Regiao
Era TB_Regiao e Agora é Regiao
</commit_message>
<xml_diff>
--- a/Estados.xlsx
+++ b/Estados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_C1A8AE7E4EF326A41D5ABDCC22D6F259B684670C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AE598B0-C694-444B-838C-A41EABE537DD}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_C1A8AE7E4EF326A41D5ABDCC22D6F259B684670C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E73A3DC-4B7B-4B5F-9460-BF8978A9CB26}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-3165" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,6 @@
     <t>Nome</t>
   </si>
   <si>
-    <t>TB Regiao</t>
-  </si>
-  <si>
     <t>AC</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>Tocantins</t>
+  </si>
+  <si>
+    <t>Regiao</t>
   </si>
 </sst>
 </file>
@@ -235,6 +235,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,7 +531,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -543,15 +547,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -559,10 +563,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -570,10 +574,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -581,10 +585,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -592,10 +596,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -603,10 +607,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -614,10 +618,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -625,10 +629,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -636,10 +640,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -647,10 +651,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -658,10 +662,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -669,10 +673,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -680,10 +684,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -691,10 +695,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -702,10 +706,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -713,10 +717,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -724,10 +728,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -735,10 +739,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -746,10 +750,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -757,10 +761,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
         <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -768,10 +772,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -779,10 +783,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -790,10 +794,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
         <v>47</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -801,10 +805,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -812,10 +816,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -823,10 +827,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
         <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -834,10 +838,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
         <v>55</v>
-      </c>
-      <c r="B28" t="s">
-        <v>56</v>
       </c>
       <c r="C28">
         <v>1</v>

</xml_diff>